<commit_message>
change done in a1 from f1
</commit_message>
<xml_diff>
--- a/a1.xlsx
+++ b/a1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>skl</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>new changes</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,6 +395,11 @@
       </c>
       <c r="F1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes commited from f2 in a1
</commit_message>
<xml_diff>
--- a/a1.xlsx
+++ b/a1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>skl</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>new changes done from f2</t>
   </si>
 </sst>
 </file>
@@ -366,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,6 +395,11 @@
       </c>
       <c r="F1" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>